<commit_message>
added some missing labels for some ontology terms
</commit_message>
<xml_diff>
--- a/ontology/doc/HaibSydhTfbs_ontology_mappings.xlsx
+++ b/ontology/doc/HaibSydhTfbs_ontology_mappings.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/ontology/EGO/ontology/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28860" windowHeight="11235" tabRatio="790" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28860" windowHeight="11240" tabRatio="790"/>
   </bookViews>
   <sheets>
     <sheet name="TF mappings" sheetId="15" r:id="rId1"/>
     <sheet name="Cell mappings" sheetId="22" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="869">
   <si>
     <t>A549</t>
   </si>
@@ -2677,12 +2682,18 @@
   <si>
     <t>http://purl.obolibrary.org/obo/CLO_0009464</t>
   </si>
+  <si>
+    <t>Pax-5</t>
+  </si>
+  <si>
+    <t>C3H zinc finger factors</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2831,28 +2842,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3179,27 +3193,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27:C32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H162" sqref="H162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
-    <col min="5" max="5" width="41.375" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" customWidth="1"/>
     <col min="6" max="6" width="49.5" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
-    <col min="8" max="8" width="24.25" customWidth="1"/>
-    <col min="9" max="9" width="25.875" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
@@ -3225,7 +3239,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>95</v>
       </c>
@@ -3243,7 +3257,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>96</v>
       </c>
@@ -3261,7 +3275,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>177</v>
       </c>
@@ -3278,7 +3292,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>190</v>
       </c>
@@ -3295,7 +3309,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>160</v>
       </c>
@@ -3312,7 +3326,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -3329,7 +3343,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>174</v>
       </c>
@@ -3346,7 +3360,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>725</v>
       </c>
@@ -3370,7 +3384,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>728</v>
       </c>
@@ -3393,7 +3407,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -3410,7 +3424,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -3427,7 +3441,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -3444,7 +3458,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>188</v>
       </c>
@@ -3464,7 +3478,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>98</v>
       </c>
@@ -3481,7 +3495,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>363</v>
       </c>
@@ -3501,7 +3515,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>157</v>
       </c>
@@ -3518,7 +3532,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>99</v>
       </c>
@@ -3535,7 +3549,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>100</v>
       </c>
@@ -3552,7 +3566,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>101</v>
       </c>
@@ -3573,7 +3587,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>62</v>
       </c>
@@ -3590,7 +3604,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>87</v>
       </c>
@@ -3608,7 +3622,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>57</v>
       </c>
@@ -3626,7 +3640,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -3643,7 +3657,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>112</v>
       </c>
@@ -3660,7 +3674,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>172</v>
       </c>
@@ -3681,7 +3695,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>56</v>
       </c>
@@ -3698,7 +3712,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>173</v>
       </c>
@@ -3715,7 +3729,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="17.25" customHeight="1">
+    <row r="29" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>105</v>
       </c>
@@ -3735,7 +3749,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>164</v>
       </c>
@@ -3752,7 +3766,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="21" customHeight="1">
+    <row r="31" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>155</v>
       </c>
@@ -3772,7 +3786,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>168</v>
       </c>
@@ -3793,7 +3807,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>142</v>
       </c>
@@ -3810,7 +3824,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>88</v>
       </c>
@@ -3827,7 +3841,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>52</v>
       </c>
@@ -3844,7 +3858,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>145</v>
       </c>
@@ -3861,7 +3875,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>102</v>
       </c>
@@ -3878,7 +3892,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -3895,7 +3909,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3912,7 +3926,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>141</v>
       </c>
@@ -3932,7 +3946,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>21</v>
       </c>
@@ -3950,7 +3964,7 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>132</v>
       </c>
@@ -3968,7 +3982,7 @@
       </c>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>176</v>
       </c>
@@ -3986,7 +4000,7 @@
       </c>
       <c r="G43" s="13"/>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>92</v>
       </c>
@@ -4003,7 +4017,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>22</v>
       </c>
@@ -4021,7 +4035,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>64</v>
       </c>
@@ -4042,7 +4056,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -4060,7 +4074,7 @@
       </c>
       <c r="G47" s="12"/>
     </row>
-    <row r="48" spans="2:9">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>165</v>
       </c>
@@ -4074,7 +4088,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>5</v>
       </c>
@@ -4088,7 +4102,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>154</v>
       </c>
@@ -4105,7 +4119,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>156</v>
       </c>
@@ -4122,7 +4136,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>159</v>
       </c>
@@ -4139,7 +4153,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>48</v>
       </c>
@@ -4156,7 +4170,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>6</v>
       </c>
@@ -4177,7 +4191,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>113</v>
       </c>
@@ -4195,7 +4209,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>110</v>
       </c>
@@ -4213,7 +4227,7 @@
       </c>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>183</v>
       </c>
@@ -4230,7 +4244,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>196</v>
       </c>
@@ -4247,7 +4261,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>133</v>
       </c>
@@ -4264,7 +4278,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>65</v>
       </c>
@@ -4284,7 +4298,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>7</v>
       </c>
@@ -4304,7 +4318,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="5" t="s">
         <v>106</v>
       </c>
@@ -4319,7 +4333,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>114</v>
       </c>
@@ -4333,7 +4347,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>151</v>
       </c>
@@ -4347,7 +4361,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>373</v>
       </c>
@@ -4365,7 +4379,7 @@
       </c>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="2:9">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>167</v>
       </c>
@@ -4382,7 +4396,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="67" spans="2:9">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4396,7 +4410,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="2:9">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>41</v>
       </c>
@@ -4414,7 +4428,7 @@
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="2:9">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>115</v>
       </c>
@@ -4431,7 +4445,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="70" spans="2:9">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>107</v>
       </c>
@@ -4448,7 +4462,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="2:9">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>179</v>
       </c>
@@ -4465,7 +4479,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="2:9">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>108</v>
       </c>
@@ -4482,7 +4496,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="2:9">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>194</v>
       </c>
@@ -4499,7 +4513,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="74" spans="2:9">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="5" t="s">
         <v>103</v>
       </c>
@@ -4519,7 +4533,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="75" spans="2:9">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>116</v>
       </c>
@@ -4536,7 +4550,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="2:9">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>66</v>
       </c>
@@ -4553,7 +4567,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="2:9">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>158</v>
       </c>
@@ -4567,7 +4581,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="78" spans="2:9">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>8</v>
       </c>
@@ -4584,7 +4598,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="79" spans="2:9">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="5" t="s">
         <v>374</v>
       </c>
@@ -4604,7 +4618,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="80" spans="2:9">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>181</v>
       </c>
@@ -4621,7 +4635,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="2:9">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -4638,7 +4652,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="2:9">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>9</v>
       </c>
@@ -4655,7 +4669,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="2:9">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>152</v>
       </c>
@@ -4673,7 +4687,7 @@
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="2:9">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>185</v>
       </c>
@@ -4687,7 +4701,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="85" spans="2:9">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>27</v>
       </c>
@@ -4704,7 +4718,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="2:9">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>161</v>
       </c>
@@ -4721,7 +4735,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="87" spans="2:9">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>187</v>
       </c>
@@ -4738,7 +4752,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="88" spans="2:9">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>137</v>
       </c>
@@ -4755,7 +4769,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="89" spans="2:9">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>198</v>
       </c>
@@ -4769,7 +4783,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="2:9">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>192</v>
       </c>
@@ -4786,7 +4800,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="91" spans="2:9">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="5" t="s">
         <v>117</v>
       </c>
@@ -4806,7 +4820,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="92" spans="2:9">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="3" t="s">
         <v>118</v>
       </c>
@@ -4827,7 +4841,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="93" spans="2:9">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="3" t="s">
         <v>67</v>
       </c>
@@ -4848,7 +4862,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="94" spans="2:9">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="3" t="s">
         <v>68</v>
       </c>
@@ -4869,7 +4883,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="95" spans="2:9">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>193</v>
       </c>
@@ -4886,7 +4900,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="2:9">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>143</v>
       </c>
@@ -4900,7 +4914,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="97" spans="2:9">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>61</v>
       </c>
@@ -4918,7 +4932,7 @@
       </c>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="2:9">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>134</v>
       </c>
@@ -4932,7 +4946,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="2:9">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>69</v>
       </c>
@@ -4949,7 +4963,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="2:9">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="3" t="s">
         <v>10</v>
       </c>
@@ -4967,7 +4981,7 @@
       </c>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="2:9">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>366</v>
       </c>
@@ -4985,16 +4999,15 @@
       </c>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="2:9">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>367</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="D102" t="e">
-        <f>VLOOKUP(C102,#REF!,2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="D102" t="s">
+        <v>867</v>
       </c>
       <c r="E102" t="s">
         <v>702</v>
@@ -5006,16 +5019,15 @@
         <v>837</v>
       </c>
     </row>
-    <row r="103" spans="2:9">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>28</v>
       </c>
       <c r="C103" t="s">
         <v>486</v>
       </c>
-      <c r="D103" t="e">
-        <f>VLOOKUP(C103,#REF!,2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="D103" t="s">
+        <v>867</v>
       </c>
       <c r="E103" t="s">
         <v>702</v>
@@ -5027,7 +5039,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="104" spans="2:9">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>11</v>
       </c>
@@ -5044,7 +5056,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="105" spans="2:9">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="5" t="s">
         <v>109</v>
       </c>
@@ -5062,7 +5074,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="106" spans="2:9">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>150</v>
       </c>
@@ -5079,7 +5091,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="107" spans="2:9">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="5" t="s">
         <v>12</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="2:9">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="5" t="s">
         <v>29</v>
       </c>
@@ -5116,7 +5128,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="109" spans="2:9">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="5" t="s">
         <v>70</v>
       </c>
@@ -5133,7 +5145,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="110" spans="2:9">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" s="8" t="s">
         <v>30</v>
       </c>
@@ -5150,7 +5162,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="111" spans="2:9">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" s="8" t="s">
         <v>149</v>
       </c>
@@ -5165,7 +5177,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="112" spans="2:9">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>144</v>
       </c>
@@ -5182,7 +5194,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="113" spans="2:9">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B113" s="3" t="s">
         <v>31</v>
       </c>
@@ -5200,7 +5212,7 @@
       </c>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="2:9">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>13</v>
       </c>
@@ -5214,7 +5226,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="115" spans="2:9">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>139</v>
       </c>
@@ -5231,7 +5243,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="116" spans="2:9">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B116" s="5" t="s">
         <v>104</v>
       </c>
@@ -5248,7 +5260,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="117" spans="2:9">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>191</v>
       </c>
@@ -5265,7 +5277,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="118" spans="2:9">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>32</v>
       </c>
@@ -5282,7 +5294,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="119" spans="2:9">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>119</v>
       </c>
@@ -5296,7 +5308,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="120" spans="2:9">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>180</v>
       </c>
@@ -5310,7 +5322,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="121" spans="2:9">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="5" t="s">
         <v>369</v>
       </c>
@@ -5330,7 +5342,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="122" spans="2:9">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -5344,7 +5356,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="123" spans="2:9">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>14</v>
       </c>
@@ -5361,7 +5373,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="124" spans="2:9">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>178</v>
       </c>
@@ -5375,7 +5387,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="125" spans="2:9">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>15</v>
       </c>
@@ -5392,7 +5404,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="126" spans="2:9">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>163</v>
       </c>
@@ -5409,7 +5421,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="127" spans="2:9">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>182</v>
       </c>
@@ -5426,7 +5438,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="128" spans="2:9">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
         <v>71</v>
       </c>
@@ -5443,7 +5455,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="129" spans="2:10">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>72</v>
       </c>
@@ -5464,7 +5476,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="130" spans="2:10">
+    <row r="130" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>73</v>
       </c>
@@ -5485,7 +5497,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="131" spans="2:10">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>23</v>
       </c>
@@ -5502,7 +5514,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="132" spans="2:10">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>74</v>
       </c>
@@ -5519,7 +5531,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="133" spans="2:10">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>121</v>
       </c>
@@ -5536,7 +5548,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="134" spans="2:10">
+    <row r="134" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>75</v>
       </c>
@@ -5553,7 +5565,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="135" spans="2:10">
+    <row r="135" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>146</v>
       </c>
@@ -5570,7 +5582,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="136" spans="2:10">
+    <row r="136" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>89</v>
       </c>
@@ -5584,7 +5596,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="137" spans="2:10">
+    <row r="137" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>16</v>
       </c>
@@ -5601,7 +5613,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="138" spans="2:10">
+    <row r="138" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>153</v>
       </c>
@@ -5615,7 +5627,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="139" spans="2:10">
+    <row r="139" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>186</v>
       </c>
@@ -5632,7 +5644,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="140" spans="2:10">
+    <row r="140" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B140" s="5" t="s">
         <v>136</v>
       </c>
@@ -5652,7 +5664,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="141" spans="2:10">
+    <row r="141" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>76</v>
       </c>
@@ -5669,7 +5681,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="142" spans="2:10">
+    <row r="142" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>17</v>
       </c>
@@ -5683,7 +5695,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="143" spans="2:10">
+    <row r="143" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>169</v>
       </c>
@@ -5697,7 +5709,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="2:10">
+    <row r="144" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>90</v>
       </c>
@@ -5714,7 +5726,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="145" spans="2:9">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>175</v>
       </c>
@@ -5728,7 +5740,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="146" spans="2:9">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B146" s="5" t="s">
         <v>370</v>
       </c>
@@ -5745,7 +5757,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="147" spans="2:9">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>199</v>
       </c>
@@ -5762,7 +5774,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="148" spans="2:9">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>77</v>
       </c>
@@ -5780,7 +5792,7 @@
       </c>
       <c r="H148" s="2"/>
     </row>
-    <row r="149" spans="2:9">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>189</v>
       </c>
@@ -5794,7 +5806,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="150" spans="2:9">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>147</v>
       </c>
@@ -5815,7 +5827,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="151" spans="2:9">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>171</v>
       </c>
@@ -5835,7 +5847,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="152" spans="2:9">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="5" t="s">
         <v>377</v>
       </c>
@@ -5855,7 +5867,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="153" spans="2:9">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>184</v>
       </c>
@@ -5872,7 +5884,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="154" spans="2:9">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>78</v>
       </c>
@@ -5889,7 +5901,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="155" spans="2:9">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B155" s="5" t="s">
         <v>79</v>
       </c>
@@ -5906,7 +5918,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="156" spans="2:9">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>122</v>
       </c>
@@ -5920,7 +5932,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="157" spans="2:9">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>35</v>
       </c>
@@ -5934,7 +5946,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="158" spans="2:9">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>19</v>
       </c>
@@ -5951,7 +5963,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="159" spans="2:9">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>140</v>
       </c>
@@ -5968,7 +5980,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="160" spans="2:9">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="6" t="s">
         <v>135</v>
       </c>
@@ -5981,15 +5993,14 @@
       <c r="G160" t="s">
         <v>415</v>
       </c>
-      <c r="H160" t="e">
-        <f>VLOOKUP(G160,#REF!,2,FALSE)</f>
-        <v>#REF!</v>
+      <c r="H160" t="s">
+        <v>868</v>
       </c>
       <c r="I160" s="5" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="161" spans="2:10">
+    <row r="161" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>195</v>
       </c>
@@ -6006,7 +6017,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="162" spans="2:10">
+    <row r="162" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>197</v>
       </c>
@@ -6023,7 +6034,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="163" spans="2:10">
+    <row r="163" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B163" s="10" t="s">
         <v>200</v>
       </c>
@@ -6046,7 +6057,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="164" spans="2:10">
+    <row r="164" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>138</v>
       </c>
@@ -6063,7 +6074,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="165" spans="2:10">
+    <row r="165" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>123</v>
       </c>
@@ -6080,7 +6091,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="166" spans="2:10">
+    <row r="166" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>94</v>
       </c>
@@ -6097,7 +6108,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="167" spans="2:10">
+    <row r="167" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>59</v>
       </c>
@@ -6114,7 +6125,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="168" spans="2:10">
+    <row r="168" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>162</v>
       </c>
@@ -6131,7 +6142,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="169" spans="2:10">
+    <row r="169" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B169" s="6" t="s">
         <v>80</v>
       </c>
@@ -6148,15 +6159,16 @@
         <v>414</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G32" r:id="rId1" location="3.5.1.2" display="http://purl.obolibrary.org/obo/TFClass_human.obo#3.5.1.2"/>
+    <hyperlink ref="C102" r:id="rId2" location="3.2.2.2.2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6166,21 +6178,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="56.25" customWidth="1"/>
-    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -6191,7 +6203,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6202,7 +6214,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -6213,7 +6225,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -6224,7 +6236,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -6235,7 +6247,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -6246,7 +6258,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -6257,7 +6269,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -6268,7 +6280,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>81</v>
       </c>
@@ -6279,7 +6291,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -6290,7 +6302,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -6301,7 +6313,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -6312,7 +6324,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -6323,7 +6335,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -6334,7 +6346,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
@@ -6345,7 +6357,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
@@ -6356,7 +6368,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -6367,7 +6379,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -6378,7 +6390,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>93</v>
       </c>
@@ -6389,7 +6401,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
@@ -6400,7 +6412,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -6411,7 +6423,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -6422,7 +6434,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -6433,7 +6445,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -6444,7 +6456,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>44</v>
       </c>
@@ -6455,7 +6467,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -6466,7 +6478,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>362</v>
       </c>
@@ -6477,7 +6489,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -6488,7 +6500,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -6499,7 +6511,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -6510,7 +6522,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>126</v>
       </c>
@@ -6521,7 +6533,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>127</v>
       </c>
@@ -6532,7 +6544,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -6543,7 +6555,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -6554,7 +6566,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -6565,7 +6577,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -6576,7 +6588,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -6587,7 +6599,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -6598,7 +6610,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -6609,7 +6621,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>130</v>
       </c>
@@ -6620,7 +6632,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
add Encode term to EGO ontology term mappings
</commit_message>
<xml_diff>
--- a/ontology/doc/HaibSydhTfbs_ontology_mappings.xlsx
+++ b/ontology/doc/HaibSydhTfbs_ontology_mappings.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28860" windowHeight="11240" tabRatio="790"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="11240" tabRatio="790" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TF mappings" sheetId="15" r:id="rId1"/>
     <sheet name="Cell mappings" sheetId="22" r:id="rId2"/>
+    <sheet name="EncodeNames to EGO terms" sheetId="23" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="893">
   <si>
     <t>A549</t>
   </si>
@@ -2687,6 +2688,78 @@
   </si>
   <si>
     <t>C3H zinc finger factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRI </t>
+  </si>
+  <si>
+    <t>Encode name</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EGO_0000000118</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0001601</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0010422</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0023758</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0022851</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0022859</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0022856</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0028068</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0024913</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0024847</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0026303</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0025875</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0027332</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0003699</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0003775</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0050126</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0007606</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0008425</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0008734</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0009015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0009058</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0009059</t>
   </si>
 </sst>
 </file>
@@ -3196,9 +3269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H162" sqref="H162"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6182,7 +6255,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B41" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6646,4 +6719,1695 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B209"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B209"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>613</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>781</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>614</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>615</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>617</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>618</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>726</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>729</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>619</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>621</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>785</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>622</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>624</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>626</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>627</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>629</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>722</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>653</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>675</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>689</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>631</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>632</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>640</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>633</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>634</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>801</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>635</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>803</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>711</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>636</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>637</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>638</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>639</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>642</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>643</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>644</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>645</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>646</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>648</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>649</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>650</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>805</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>651</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>652</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>655</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>656</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>657</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>658</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>659</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>660</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>809</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>661</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>662</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>661</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>662</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>663</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>678</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>699</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>871</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>664</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>815</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>642</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>665</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>666</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>818</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>667</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>668</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>669</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>670</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>671</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>820</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>672</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>673</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>674</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>677</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>761</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>680</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>681</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>682</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>823</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>683</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>684</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>685</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>686</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>687</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>688</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>691</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>824</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>693</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>828</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>830</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>692</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>695</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>834</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>698</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>701</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>713</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>836</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>702</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>702</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>704</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>839</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>705</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>841</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>841</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>844</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>708</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>846</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>709</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>735</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>710</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>715</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>706</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>716</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>717</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>718</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>719</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>719</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>720</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>721</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>731</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>732</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>733</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>734</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>748</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>738</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>741</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>743</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>744</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>745</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>746</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>747</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>750</v>
+      </c>
+      <c r="B136" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>751</v>
+      </c>
+      <c r="B137" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>752</v>
+      </c>
+      <c r="B138" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>753</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>754</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>755</v>
+      </c>
+      <c r="B141" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>756</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>757</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>758</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>759</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>793</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>760</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>696</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>761</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>762</v>
+      </c>
+      <c r="B150" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>762</v>
+      </c>
+      <c r="B151" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>763</v>
+      </c>
+      <c r="B152" s="16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>763</v>
+      </c>
+      <c r="B153" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>764</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>765</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>766</v>
+      </c>
+      <c r="B156" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>767</v>
+      </c>
+      <c r="B157" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>768</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>769</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>788</v>
+      </c>
+      <c r="B160" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>770</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>771</v>
+      </c>
+      <c r="B162" s="16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>772</v>
+      </c>
+      <c r="B163" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>774</v>
+      </c>
+      <c r="B164" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>775</v>
+      </c>
+      <c r="B165" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>776</v>
+      </c>
+      <c r="B166" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>777</v>
+      </c>
+      <c r="B167" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>778</v>
+      </c>
+      <c r="B168" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>779</v>
+      </c>
+      <c r="B169" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="B170" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>849</v>
+      </c>
+      <c r="B171" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="B172" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="9" t="s">
+        <v>874</v>
+      </c>
+      <c r="B173" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="B174" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="9" t="s">
+        <v>877</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="9" t="s">
+        <v>878</v>
+      </c>
+      <c r="B177" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="9" t="s">
+        <v>879</v>
+      </c>
+      <c r="B178" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="B179" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="9" t="s">
+        <v>881</v>
+      </c>
+      <c r="B180" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="9" t="s">
+        <v>882</v>
+      </c>
+      <c r="B181" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="9" t="s">
+        <v>883</v>
+      </c>
+      <c r="B182" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>850</v>
+      </c>
+      <c r="B183" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>851</v>
+      </c>
+      <c r="B184" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>607</v>
+      </c>
+      <c r="B185" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>852</v>
+      </c>
+      <c r="B186" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>853</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>854</v>
+      </c>
+      <c r="B189" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="B190" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>855</v>
+      </c>
+      <c r="B191" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>856</v>
+      </c>
+      <c r="B192" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="B193" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="B194" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>857</v>
+      </c>
+      <c r="B195" s="16" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>858</v>
+      </c>
+      <c r="B196" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>859</v>
+      </c>
+      <c r="B197" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>860</v>
+      </c>
+      <c r="B198" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>861</v>
+      </c>
+      <c r="B199" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>862</v>
+      </c>
+      <c r="B200" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="B201" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="9" t="s">
+        <v>889</v>
+      </c>
+      <c r="B202" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="9" t="s">
+        <v>890</v>
+      </c>
+      <c r="B203" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="9" t="s">
+        <v>891</v>
+      </c>
+      <c r="B204" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="9" t="s">
+        <v>892</v>
+      </c>
+      <c r="B205" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>863</v>
+      </c>
+      <c r="B206" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>864</v>
+      </c>
+      <c r="B207" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>865</v>
+      </c>
+      <c r="B208" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>866</v>
+      </c>
+      <c r="B209" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>